<commit_message>
Modify Test Cases : Apps Module
TC : 1.54 - Unwanted steps deleted > Changes in main test case sheet
TC : 1.26 - stabilized more fixes  > Changes in Common sheet
</commit_message>
<xml_diff>
--- a/ObjectRepository/ObjectRepository.xlsx
+++ b/ObjectRepository/ObjectRepository.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404">
   <si>
     <t>sl_no</t>
   </si>
@@ -237,7 +237,7 @@
     <t>FirstAppActionArrow</t>
   </si>
   <si>
-    <t>//td[7]/div/label</t>
+    <t>//td[7]/div/label | //td[7]/div/input</t>
   </si>
   <si>
     <t>DeletePage</t>
@@ -1282,6 +1282,27 @@
   </si>
   <si>
     <t>//div[@title='CPC']</t>
+  </si>
+  <si>
+    <t>FirstArrowButton</t>
+  </si>
+  <si>
+    <t>//table[@id='DataTables_Table_0']/tbody/tr[1]/td[8]/div/label</t>
+  </si>
+  <si>
+    <t>ArrowPopup</t>
+  </si>
+  <si>
+    <t>//li[2]/div</t>
+  </si>
+  <si>
+    <t>CancelCampaignPage</t>
+  </si>
+  <si>
+    <t>FirstCampaign</t>
+  </si>
+  <si>
+    <t>//table[@id='DataTables_Table_0']/tbody/tr[2]/td[1]/div/div[1]</t>
   </si>
 </sst>
 </file>
@@ -1289,10 +1310,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -1378,13 +1399,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="17"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="58"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1406,17 +1420,24 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color indexed="56"/>
-      <name val="Cambria"/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="Calibri"/>
+      <sz val="18"/>
+      <color indexed="56"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
@@ -1459,16 +1480,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color indexed="56"/>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="39"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="60"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="56"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -1512,21 +1548,6 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="39"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="26">
     <fill>
@@ -1549,8 +1570,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="42"/>
         <bgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -1561,14 +1594,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="13"/>
+        <fgColor indexed="45"/>
+        <bgColor indexed="29"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-        <bgColor indexed="29"/>
+        <fgColor indexed="22"/>
+        <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+        <bgColor indexed="22"/>
       </patternFill>
     </fill>
     <fill>
@@ -1585,37 +1624,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor indexed="41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="30"/>
         <bgColor indexed="21"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-        <bgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="27"/>
-        <bgColor indexed="41"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="47"/>
-        <bgColor indexed="22"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
         <bgColor indexed="22"/>
       </patternFill>
     </fill>
@@ -1633,14 +1654,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="49"/>
-        <bgColor indexed="40"/>
+        <fgColor indexed="43"/>
+        <bgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="26"/>
+        <fgColor indexed="26"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="60"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+        <bgColor indexed="40"/>
       </patternFill>
     </fill>
     <fill>
@@ -1665,18 +1698,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="55"/>
         <bgColor indexed="23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
-        <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="60"/>
       </patternFill>
     </fill>
   </fills>
@@ -1743,6 +1764,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1795,36 +1831,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="22"/>
-      </left>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1839,179 +1860,179 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2570,9 +2591,9 @@
   <dimension ref="A1:L3654"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H192" sqref="H192"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -6805,21 +6826,93 @@
         <v>396</v>
       </c>
     </row>
-    <row r="194" spans="4:5">
+    <row r="194" spans="1:8">
+      <c r="A194" s="8">
+        <v>192</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>397</v>
+      </c>
       <c r="D194" s="8"/>
       <c r="E194" s="8"/>
-    </row>
-    <row r="195" spans="4:5">
+      <c r="F194" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G194" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H194" s="8" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" s="8">
+        <v>193</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="D195" s="8"/>
       <c r="E195" s="8"/>
-    </row>
-    <row r="196" spans="4:5">
+      <c r="F195" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G195" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H195" s="8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196" s="8">
+        <v>194</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C196" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D196" s="8"/>
       <c r="E196" s="8"/>
-    </row>
-    <row r="197" spans="4:5">
+      <c r="F196" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G196" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H196" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" s="8">
+        <v>195</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>402</v>
+      </c>
       <c r="D197" s="8"/>
       <c r="E197" s="8"/>
+      <c r="F197" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G197" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H197" s="8" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="198" spans="4:5">
       <c r="D198" s="8"/>

</xml_diff>